<commit_message>
Updated uganda config file and how yaml is read. Also added flag to re-write lndu realloc factor
</commit_message>
<xml_diff>
--- a/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ce_calibrated.xlsx
+++ b/ssp_modeling/transformations/templates/calibrated/uganda/model_input_variables_uganda_ce_calibrated.xlsx
@@ -7919,112 +7919,112 @@
         <v>1</v>
       </c>
       <c r="J56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="K56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="L56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="M56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="N56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="O56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="P56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Q56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="R56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="S56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="T56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="U56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="V56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="W56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="X56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Y56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Z56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AA56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AB56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AC56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AD56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AE56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AF56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AG56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AH56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AI56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AJ56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AK56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AL56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AM56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AN56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AO56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AP56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AQ56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AR56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AS56">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
     </row>
     <row r="57" spans="1:45">
@@ -8041,112 +8041,112 @@
         <v>1</v>
       </c>
       <c r="J57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="K57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="L57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="M57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="N57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="O57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="P57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Q57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="R57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="S57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="T57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="U57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="V57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="W57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="X57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Y57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Z57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AA57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AB57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AC57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AD57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AE57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AF57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AG57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AH57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AI57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AJ57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AK57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AL57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AM57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AN57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AO57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AP57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AQ57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AR57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AS57">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
     </row>
     <row r="58" spans="1:45">
@@ -8163,112 +8163,112 @@
         <v>1</v>
       </c>
       <c r="J58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="K58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="L58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="M58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="N58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="O58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="P58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Q58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="R58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="S58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="T58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="U58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="V58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="W58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="X58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Y58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="Z58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AA58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AB58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AC58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AD58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AE58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AF58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AG58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AH58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AI58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AJ58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AK58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AL58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AM58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AN58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AO58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AP58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AQ58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AR58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
       <c r="AS58">
-        <v>0.0004199999999999</v>
+        <v>0.00042</v>
       </c>
     </row>
     <row r="59" spans="1:45">
@@ -13668,112 +13668,112 @@
         <v>1</v>
       </c>
       <c r="J103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="X103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Y103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Z103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AA103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AB103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AC103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AD103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AE103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AF103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AG103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AH103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AI103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AJ103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AK103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AL103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AM103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AN103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AO103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AP103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AQ103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AR103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AS103">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
     </row>
     <row r="104" spans="1:45">
@@ -13790,112 +13790,112 @@
         <v>1</v>
       </c>
       <c r="J104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="X104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Y104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Z104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AA104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AB104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AC104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AD104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AE104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AF104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AG104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AH104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AI104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AJ104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AK104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AL104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AM104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AN104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AO104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AP104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AQ104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AR104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AS104">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
     </row>
     <row r="105" spans="1:45">
@@ -13915,112 +13915,112 @@
         <v>1</v>
       </c>
       <c r="J105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="X105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Y105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Z105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AA105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AB105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AC105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AD105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AE105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AF105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AG105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AH105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AI105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AJ105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AK105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AL105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AM105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AN105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AO105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AP105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AQ105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AR105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AS105">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
     </row>
     <row r="106" spans="1:45">
@@ -14040,112 +14040,112 @@
         <v>1</v>
       </c>
       <c r="J106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="X106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Y106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Z106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AA106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AB106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AC106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AD106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AE106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AF106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AG106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AH106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AI106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AJ106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AK106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AL106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AM106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AN106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AO106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AP106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AQ106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AR106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="AS106">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
     </row>
     <row r="107" spans="1:45">
@@ -16724,112 +16724,112 @@
         <v>1</v>
       </c>
       <c r="J128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="K128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="L128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="M128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="N128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="O128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="P128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="Q128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="R128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="S128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="T128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="U128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="V128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="W128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="X128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="Y128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="Z128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AA128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AB128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AC128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AD128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AE128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AF128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AG128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AH128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AI128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AJ128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AK128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AL128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AM128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AN128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AO128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AP128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AQ128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AR128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
       <c r="AS128">
-        <v>0.0262446761496392</v>
+        <v>0.026244676</v>
       </c>
     </row>
     <row r="129" spans="1:45">
@@ -17090,112 +17090,112 @@
         <v>1</v>
       </c>
       <c r="J131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="K131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="L131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="M131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="N131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="O131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="P131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="Q131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="R131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="S131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="T131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="U131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="V131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="W131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="X131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="Y131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="Z131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AA131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AB131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AC131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AD131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AE131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AF131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AG131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AH131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AI131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AJ131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AK131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AL131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AM131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AN131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AO131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AP131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AQ131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AR131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
       <c r="AS131">
-        <v>0.0290245012466082</v>
+        <v>0.029024501</v>
       </c>
     </row>
     <row r="132" spans="1:45">
@@ -17212,112 +17212,112 @@
         <v>1</v>
       </c>
       <c r="J132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="K132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="L132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="M132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="N132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="O132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="P132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="Q132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="R132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="S132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="T132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="U132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="V132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="W132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="X132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="Y132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="Z132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AA132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AB132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AC132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AD132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AE132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AF132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AG132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AH132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AI132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AJ132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AK132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AL132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AM132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AN132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AO132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AP132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AQ132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AR132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
       <c r="AS132">
-        <v>0.130838334519746</v>
+        <v>0.130838335</v>
       </c>
     </row>
     <row r="133" spans="1:45">
@@ -17337,112 +17337,112 @@
         <v>1</v>
       </c>
       <c r="J133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="K133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="L133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="M133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="N133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="O133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="P133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Q133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="R133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="S133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="T133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="U133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="V133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="W133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="X133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Y133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Z133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AA133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AB133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AC133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AD133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AE133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AF133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AG133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AH133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AI133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AJ133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AK133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AL133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AM133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AN133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AO133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AP133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AQ133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AR133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AS133">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
     </row>
     <row r="134" spans="1:45">
@@ -17712,112 +17712,112 @@
         <v>1</v>
       </c>
       <c r="J136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="K136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="L136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="M136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="N136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="O136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="P136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Q136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="R136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="S136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="T136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="U136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="V136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="W136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="X136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Y136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Z136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AA136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AB136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AC136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AD136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AE136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AF136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AG136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AH136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AI136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AJ136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AK136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AL136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AM136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AN136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AO136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AP136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AQ136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AR136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="AS136">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
     </row>
     <row r="137" spans="1:45">
@@ -17837,112 +17837,112 @@
         <v>1</v>
       </c>
       <c r="J137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="K137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="L137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="M137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="N137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="O137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="P137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="Q137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="R137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="S137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="T137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="U137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="V137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="W137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="X137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="Y137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="Z137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AA137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AB137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AC137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AD137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AE137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AF137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AG137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AH137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AI137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AJ137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AK137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AL137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AM137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AN137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AO137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AP137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AQ137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AR137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
       <c r="AS137">
-        <v>0.1440108499374283</v>
+        <v>0.14401085</v>
       </c>
     </row>
     <row r="138" spans="1:45">
@@ -18087,112 +18087,112 @@
         <v>1</v>
       </c>
       <c r="J139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="K139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="L139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="M139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="N139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="O139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="P139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="Q139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="R139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="S139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="T139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="U139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="V139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="W139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="X139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="Y139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="Z139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AA139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AB139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AC139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AD139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AE139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AF139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AG139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AH139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AI139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AJ139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AK139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AL139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AM139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AN139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AO139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AP139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AQ139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AR139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="AS139">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
     </row>
     <row r="140" spans="1:45">
@@ -30509,109 +30509,109 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="K14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="L14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="M14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="N14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="O14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="P14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Q14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="R14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="S14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="T14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="U14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="V14">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="W14">
-        <v>0.07660990205985765</v>
+        <v>0.07660990234782608</v>
       </c>
       <c r="X14">
-        <v>0.1117639974207732</v>
+        <v>0.1117639976956522</v>
       </c>
       <c r="Y14">
-        <v>0.1469180927816888</v>
+        <v>0.1469180930434782</v>
       </c>
       <c r="Z14">
-        <v>0.1820721881426043</v>
+        <v>0.1820721883913043</v>
       </c>
       <c r="AA14">
-        <v>0.2172262835035199</v>
+        <v>0.2172262837391304</v>
       </c>
       <c r="AB14">
-        <v>0.2523803788644355</v>
+        <v>0.2523803790869565</v>
       </c>
       <c r="AC14">
-        <v>0.2875344742253511</v>
+        <v>0.2875344744347826</v>
       </c>
       <c r="AD14">
-        <v>0.3226885695862666</v>
+        <v>0.3226885697826086</v>
       </c>
       <c r="AE14">
-        <v>0.3578426649471822</v>
+        <v>0.3578426651304348</v>
       </c>
       <c r="AF14">
-        <v>0.3929967603080977</v>
+        <v>0.3929967604782608</v>
       </c>
       <c r="AG14">
-        <v>0.4281508556690132</v>
+        <v>0.4281508558260869</v>
       </c>
       <c r="AH14">
-        <v>0.4633049510299288</v>
+        <v>0.463304951173913</v>
       </c>
       <c r="AI14">
-        <v>0.4984590463908443</v>
+        <v>0.4984590465217391</v>
       </c>
       <c r="AJ14">
-        <v>0.53361314175176</v>
+        <v>0.5336131418695652</v>
       </c>
       <c r="AK14">
-        <v>0.5687672371126755</v>
+        <v>0.5687672372173913</v>
       </c>
       <c r="AL14">
-        <v>0.603921332473591</v>
+        <v>0.6039213325652173</v>
       </c>
       <c r="AM14">
-        <v>0.6390754278345065</v>
+        <v>0.6390754279130434</v>
       </c>
       <c r="AN14">
-        <v>0.6742295231954223</v>
+        <v>0.6742295232608696</v>
       </c>
       <c r="AO14">
-        <v>0.7093836185563377</v>
+        <v>0.7093836186086956</v>
       </c>
       <c r="AP14">
-        <v>0.7445377139172533</v>
+        <v>0.7445377139565217</v>
       </c>
       <c r="AQ14">
-        <v>0.7796918092781688</v>
+        <v>0.7796918093043478</v>
       </c>
       <c r="AR14">
-        <v>0.8148459046390845</v>
+        <v>0.8148459046521739</v>
       </c>
       <c r="AS14">
         <v>0.85</v>
@@ -30884,109 +30884,109 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="K17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="L17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="M17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="N17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="O17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="P17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Q17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="R17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="S17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="T17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="U17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="V17">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="W17">
-        <v>0.07660990205985765</v>
+        <v>0.07660990234782608</v>
       </c>
       <c r="X17">
-        <v>0.1117639974207732</v>
+        <v>0.1117639976956522</v>
       </c>
       <c r="Y17">
-        <v>0.1469180927816888</v>
+        <v>0.1469180930434782</v>
       </c>
       <c r="Z17">
-        <v>0.1820721881426043</v>
+        <v>0.1820721883913043</v>
       </c>
       <c r="AA17">
-        <v>0.2172262835035199</v>
+        <v>0.2172262837391304</v>
       </c>
       <c r="AB17">
-        <v>0.2523803788644355</v>
+        <v>0.2523803790869565</v>
       </c>
       <c r="AC17">
-        <v>0.2875344742253511</v>
+        <v>0.2875344744347826</v>
       </c>
       <c r="AD17">
-        <v>0.3226885695862666</v>
+        <v>0.3226885697826086</v>
       </c>
       <c r="AE17">
-        <v>0.3578426649471822</v>
+        <v>0.3578426651304348</v>
       </c>
       <c r="AF17">
-        <v>0.3929967603080977</v>
+        <v>0.3929967604782608</v>
       </c>
       <c r="AG17">
-        <v>0.4281508556690132</v>
+        <v>0.4281508558260869</v>
       </c>
       <c r="AH17">
-        <v>0.4633049510299288</v>
+        <v>0.463304951173913</v>
       </c>
       <c r="AI17">
-        <v>0.4984590463908443</v>
+        <v>0.4984590465217391</v>
       </c>
       <c r="AJ17">
-        <v>0.53361314175176</v>
+        <v>0.5336131418695652</v>
       </c>
       <c r="AK17">
-        <v>0.5687672371126755</v>
+        <v>0.5687672372173913</v>
       </c>
       <c r="AL17">
-        <v>0.603921332473591</v>
+        <v>0.6039213325652173</v>
       </c>
       <c r="AM17">
-        <v>0.6390754278345065</v>
+        <v>0.6390754279130434</v>
       </c>
       <c r="AN17">
-        <v>0.6742295231954223</v>
+        <v>0.6742295232608696</v>
       </c>
       <c r="AO17">
-        <v>0.7093836185563377</v>
+        <v>0.7093836186086956</v>
       </c>
       <c r="AP17">
-        <v>0.7445377139172533</v>
+        <v>0.7445377139565217</v>
       </c>
       <c r="AQ17">
-        <v>0.7796918092781688</v>
+        <v>0.7796918093043478</v>
       </c>
       <c r="AR17">
-        <v>0.8148459046390845</v>
+        <v>0.8148459046521739</v>
       </c>
       <c r="AS17">
         <v>0.85</v>
@@ -31134,112 +31134,112 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="K19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="L19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="M19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="N19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="O19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="P19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="Q19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="R19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="S19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="T19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="U19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="V19">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="W19">
-        <v>0.8342500196277892</v>
+        <v>0.8342500195652174</v>
       </c>
       <c r="X19">
-        <v>0.8125108891930065</v>
+        <v>0.8125108891304348</v>
       </c>
       <c r="Y19">
-        <v>0.7907717587582239</v>
+        <v>0.7907717586956521</v>
       </c>
       <c r="Z19">
-        <v>0.7690326283234412</v>
+        <v>0.7690326282608696</v>
       </c>
       <c r="AA19">
-        <v>0.7472934978886587</v>
+        <v>0.747293497826087</v>
       </c>
       <c r="AB19">
-        <v>0.7255543674538759</v>
+        <v>0.7255543673913042</v>
       </c>
       <c r="AC19">
-        <v>0.7038152370190934</v>
+        <v>0.7038152369565217</v>
       </c>
       <c r="AD19">
-        <v>0.6820761065843108</v>
+        <v>0.6820761065217391</v>
       </c>
       <c r="AE19">
-        <v>0.6603369761495282</v>
+        <v>0.6603369760869566</v>
       </c>
       <c r="AF19">
-        <v>0.6385978457147456</v>
+        <v>0.6385978456521739</v>
       </c>
       <c r="AG19">
-        <v>0.6168587152799629</v>
+        <v>0.6168587152173912</v>
       </c>
       <c r="AH19">
-        <v>0.5951195848451805</v>
+        <v>0.5951195847826087</v>
       </c>
       <c r="AI19">
-        <v>0.5733804544103979</v>
+        <v>0.573380454347826</v>
       </c>
       <c r="AJ19">
-        <v>0.5516413239756152</v>
+        <v>0.5516413239130434</v>
       </c>
       <c r="AK19">
-        <v>0.5299021935408326</v>
+        <v>0.5299021934782608</v>
       </c>
       <c r="AL19">
-        <v>0.50816306310605</v>
+        <v>0.5081630630434782</v>
       </c>
       <c r="AM19">
-        <v>0.4864239326712674</v>
+        <v>0.4864239326086957</v>
       </c>
       <c r="AN19">
-        <v>0.4646848022364848</v>
+        <v>0.4646848021739129</v>
       </c>
       <c r="AO19">
-        <v>0.4429456718017022</v>
+        <v>0.4429456717391304</v>
       </c>
       <c r="AP19">
-        <v>0.4212065413669195</v>
+        <v>0.4212065413043478</v>
       </c>
       <c r="AQ19">
-        <v>0.3994674109321369</v>
+        <v>0.3994674108695652</v>
       </c>
       <c r="AR19">
-        <v>0.3777282804973543</v>
+        <v>0.3777282804347826</v>
       </c>
       <c r="AS19">
-        <v>0.3559891500625717</v>
+        <v>0.35598915</v>
       </c>
     </row>
     <row r="20" spans="1:45">
@@ -34281,109 +34281,109 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V17">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W17">
-        <v>0.02624921922445162</v>
+        <v>0.02624921878260869</v>
       </c>
       <c r="X17">
-        <v>0.04664698198697655</v>
+        <v>0.04664698156521739</v>
       </c>
       <c r="Y17">
-        <v>0.06704474474950148</v>
+        <v>0.06704474434782608</v>
       </c>
       <c r="Z17">
-        <v>0.0874425075120264</v>
+        <v>0.08744250713043478</v>
       </c>
       <c r="AA17">
-        <v>0.1078402702745513</v>
+        <v>0.1078402699130435</v>
       </c>
       <c r="AB17">
-        <v>0.1282380330370763</v>
+        <v>0.1282380326956522</v>
       </c>
       <c r="AC17">
-        <v>0.1486357957996012</v>
+        <v>0.1486357954782609</v>
       </c>
       <c r="AD17">
-        <v>0.1690335585621261</v>
+        <v>0.1690335582608695</v>
       </c>
       <c r="AE17">
-        <v>0.189431321324651</v>
+        <v>0.1894313210434783</v>
       </c>
       <c r="AF17">
-        <v>0.2098290840871759</v>
+        <v>0.2098290838260869</v>
       </c>
       <c r="AG17">
-        <v>0.2302268468497009</v>
+        <v>0.2302268466086956</v>
       </c>
       <c r="AH17">
-        <v>0.2506246096122258</v>
+        <v>0.2506246093913043</v>
       </c>
       <c r="AI17">
-        <v>0.2710223723747507</v>
+        <v>0.271022372173913</v>
       </c>
       <c r="AJ17">
-        <v>0.2914201351372757</v>
+        <v>0.2914201349565217</v>
       </c>
       <c r="AK17">
-        <v>0.3118178978998006</v>
+        <v>0.3118178977391304</v>
       </c>
       <c r="AL17">
-        <v>0.3322156606623255</v>
+        <v>0.3322156605217391</v>
       </c>
       <c r="AM17">
-        <v>0.3526134234248504</v>
+        <v>0.3526134233043478</v>
       </c>
       <c r="AN17">
-        <v>0.3730111861873754</v>
+        <v>0.3730111860869565</v>
       </c>
       <c r="AO17">
-        <v>0.3934089489499003</v>
+        <v>0.3934089488695652</v>
       </c>
       <c r="AP17">
-        <v>0.4138067117124252</v>
+        <v>0.4138067116521739</v>
       </c>
       <c r="AQ17">
-        <v>0.4342044744749501</v>
+        <v>0.4342044744347826</v>
       </c>
       <c r="AR17">
-        <v>0.4546022372374751</v>
+        <v>0.4546022372173913</v>
       </c>
       <c r="AS17">
         <v>0.475</v>
@@ -34406,109 +34406,109 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V18">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W18">
-        <v>0.02624921922445162</v>
+        <v>0.02624921878260869</v>
       </c>
       <c r="X18">
-        <v>0.04664698198697655</v>
+        <v>0.04664698156521739</v>
       </c>
       <c r="Y18">
-        <v>0.06704474474950148</v>
+        <v>0.06704474434782608</v>
       </c>
       <c r="Z18">
-        <v>0.0874425075120264</v>
+        <v>0.08744250713043478</v>
       </c>
       <c r="AA18">
-        <v>0.1078402702745513</v>
+        <v>0.1078402699130435</v>
       </c>
       <c r="AB18">
-        <v>0.1282380330370763</v>
+        <v>0.1282380326956522</v>
       </c>
       <c r="AC18">
-        <v>0.1486357957996012</v>
+        <v>0.1486357954782609</v>
       </c>
       <c r="AD18">
-        <v>0.1690335585621261</v>
+        <v>0.1690335582608695</v>
       </c>
       <c r="AE18">
-        <v>0.189431321324651</v>
+        <v>0.1894313210434783</v>
       </c>
       <c r="AF18">
-        <v>0.2098290840871759</v>
+        <v>0.2098290838260869</v>
       </c>
       <c r="AG18">
-        <v>0.2302268468497009</v>
+        <v>0.2302268466086956</v>
       </c>
       <c r="AH18">
-        <v>0.2506246096122258</v>
+        <v>0.2506246093913043</v>
       </c>
       <c r="AI18">
-        <v>0.2710223723747507</v>
+        <v>0.271022372173913</v>
       </c>
       <c r="AJ18">
-        <v>0.2914201351372757</v>
+        <v>0.2914201349565217</v>
       </c>
       <c r="AK18">
-        <v>0.3118178978998006</v>
+        <v>0.3118178977391304</v>
       </c>
       <c r="AL18">
-        <v>0.3322156606623255</v>
+        <v>0.3322156605217391</v>
       </c>
       <c r="AM18">
-        <v>0.3526134234248504</v>
+        <v>0.3526134233043478</v>
       </c>
       <c r="AN18">
-        <v>0.3730111861873754</v>
+        <v>0.3730111860869565</v>
       </c>
       <c r="AO18">
-        <v>0.3934089489499003</v>
+        <v>0.3934089488695652</v>
       </c>
       <c r="AP18">
-        <v>0.4138067117124252</v>
+        <v>0.4138067116521739</v>
       </c>
       <c r="AQ18">
-        <v>0.4342044744749501</v>
+        <v>0.4342044744347826</v>
       </c>
       <c r="AR18">
-        <v>0.4546022372374751</v>
+        <v>0.4546022372173913</v>
       </c>
       <c r="AS18">
         <v>0.475</v>
@@ -34531,109 +34531,109 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="K19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="L19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="M19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="N19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="O19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="P19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="Q19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="R19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="S19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="T19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="U19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="V19">
-        <v>0.0058514564619267</v>
+        <v>0.005851456</v>
       </c>
       <c r="W19">
-        <v>0.02624921922445162</v>
+        <v>0.02624921878260869</v>
       </c>
       <c r="X19">
-        <v>0.04664698198697655</v>
+        <v>0.04664698156521739</v>
       </c>
       <c r="Y19">
-        <v>0.06704474474950148</v>
+        <v>0.06704474434782608</v>
       </c>
       <c r="Z19">
-        <v>0.0874425075120264</v>
+        <v>0.08744250713043478</v>
       </c>
       <c r="AA19">
-        <v>0.1078402702745513</v>
+        <v>0.1078402699130435</v>
       </c>
       <c r="AB19">
-        <v>0.1282380330370763</v>
+        <v>0.1282380326956522</v>
       </c>
       <c r="AC19">
-        <v>0.1486357957996012</v>
+        <v>0.1486357954782609</v>
       </c>
       <c r="AD19">
-        <v>0.1690335585621261</v>
+        <v>0.1690335582608695</v>
       </c>
       <c r="AE19">
-        <v>0.189431321324651</v>
+        <v>0.1894313210434783</v>
       </c>
       <c r="AF19">
-        <v>0.2098290840871759</v>
+        <v>0.2098290838260869</v>
       </c>
       <c r="AG19">
-        <v>0.2302268468497009</v>
+        <v>0.2302268466086956</v>
       </c>
       <c r="AH19">
-        <v>0.2506246096122258</v>
+        <v>0.2506246093913043</v>
       </c>
       <c r="AI19">
-        <v>0.2710223723747507</v>
+        <v>0.271022372173913</v>
       </c>
       <c r="AJ19">
-        <v>0.2914201351372757</v>
+        <v>0.2914201349565217</v>
       </c>
       <c r="AK19">
-        <v>0.3118178978998006</v>
+        <v>0.3118178977391304</v>
       </c>
       <c r="AL19">
-        <v>0.3322156606623255</v>
+        <v>0.3322156605217391</v>
       </c>
       <c r="AM19">
-        <v>0.3526134234248504</v>
+        <v>0.3526134233043478</v>
       </c>
       <c r="AN19">
-        <v>0.3730111861873754</v>
+        <v>0.3730111860869565</v>
       </c>
       <c r="AO19">
-        <v>0.3934089489499003</v>
+        <v>0.3934089488695652</v>
       </c>
       <c r="AP19">
-        <v>0.4138067117124252</v>
+        <v>0.4138067116521739</v>
       </c>
       <c r="AQ19">
-        <v>0.4342044744749501</v>
+        <v>0.4342044744347826</v>
       </c>
       <c r="AR19">
-        <v>0.4546022372374751</v>
+        <v>0.4546022372173913</v>
       </c>
       <c r="AS19">
         <v>0.475</v>
@@ -34656,109 +34656,109 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="K20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="L20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="M20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="N20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="O20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="P20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Q20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="R20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="S20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="T20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="U20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="V20">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="W20">
-        <v>0.08313164119029245</v>
+        <v>0.08313164147826087</v>
       </c>
       <c r="X20">
-        <v>0.1248074756816428</v>
+        <v>0.1248074759565217</v>
       </c>
       <c r="Y20">
-        <v>0.1664833101729931</v>
+        <v>0.1664833104347826</v>
       </c>
       <c r="Z20">
-        <v>0.2081591446643435</v>
+        <v>0.2081591449130435</v>
       </c>
       <c r="AA20">
-        <v>0.2498349791556938</v>
+        <v>0.2498349793913043</v>
       </c>
       <c r="AB20">
-        <v>0.2915108136470442</v>
+        <v>0.2915108138695652</v>
       </c>
       <c r="AC20">
-        <v>0.3331866481383945</v>
+        <v>0.3331866483478261</v>
       </c>
       <c r="AD20">
-        <v>0.3748624826297449</v>
+        <v>0.3748624828260869</v>
       </c>
       <c r="AE20">
-        <v>0.4165383171210952</v>
+        <v>0.4165383173043479</v>
       </c>
       <c r="AF20">
-        <v>0.4582141516124456</v>
+        <v>0.4582141517826087</v>
       </c>
       <c r="AG20">
-        <v>0.4998899861037959</v>
+        <v>0.4998899862608696</v>
       </c>
       <c r="AH20">
-        <v>0.5415658205951462</v>
+        <v>0.5415658207391304</v>
       </c>
       <c r="AI20">
-        <v>0.5832416550864965</v>
+        <v>0.5832416552173912</v>
       </c>
       <c r="AJ20">
-        <v>0.624917489577847</v>
+        <v>0.6249174896956522</v>
       </c>
       <c r="AK20">
-        <v>0.6665933240691972</v>
+        <v>0.666593324173913</v>
       </c>
       <c r="AL20">
-        <v>0.7082691585605476</v>
+        <v>0.7082691586521739</v>
       </c>
       <c r="AM20">
-        <v>0.7499449930518979</v>
+        <v>0.7499449931304347</v>
       </c>
       <c r="AN20">
-        <v>0.7916208275432484</v>
+        <v>0.7916208276086957</v>
       </c>
       <c r="AO20">
-        <v>0.8332966620345986</v>
+        <v>0.8332966620869565</v>
       </c>
       <c r="AP20">
-        <v>0.874972496525949</v>
+        <v>0.8749724965652174</v>
       </c>
       <c r="AQ20">
-        <v>0.9166483310172993</v>
+        <v>0.9166483310434782</v>
       </c>
       <c r="AR20">
-        <v>0.9583241655086497</v>
+        <v>0.9583241655217392</v>
       </c>
       <c r="AS20">
         <v>1</v>
@@ -35031,109 +35031,109 @@
         <v>1</v>
       </c>
       <c r="J23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="K23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="L23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="M23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="N23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="O23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="P23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="Q23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="R23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="S23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="T23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="U23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="V23">
-        <v>0.0414558066989421</v>
+        <v>0.041455807</v>
       </c>
       <c r="W23">
-        <v>0.08313164119029245</v>
+        <v>0.08313164147826087</v>
       </c>
       <c r="X23">
-        <v>0.1248074756816428</v>
+        <v>0.1248074759565217</v>
       </c>
       <c r="Y23">
-        <v>0.1664833101729931</v>
+        <v>0.1664833104347826</v>
       </c>
       <c r="Z23">
-        <v>0.2081591446643435</v>
+        <v>0.2081591449130435</v>
       </c>
       <c r="AA23">
-        <v>0.2498349791556938</v>
+        <v>0.2498349793913043</v>
       </c>
       <c r="AB23">
-        <v>0.2915108136470442</v>
+        <v>0.2915108138695652</v>
       </c>
       <c r="AC23">
-        <v>0.3331866481383945</v>
+        <v>0.3331866483478261</v>
       </c>
       <c r="AD23">
-        <v>0.3748624826297449</v>
+        <v>0.3748624828260869</v>
       </c>
       <c r="AE23">
-        <v>0.4165383171210952</v>
+        <v>0.4165383173043479</v>
       </c>
       <c r="AF23">
-        <v>0.4582141516124456</v>
+        <v>0.4582141517826087</v>
       </c>
       <c r="AG23">
-        <v>0.4998899861037959</v>
+        <v>0.4998899862608696</v>
       </c>
       <c r="AH23">
-        <v>0.5415658205951462</v>
+        <v>0.5415658207391304</v>
       </c>
       <c r="AI23">
-        <v>0.5832416550864965</v>
+        <v>0.5832416552173912</v>
       </c>
       <c r="AJ23">
-        <v>0.624917489577847</v>
+        <v>0.6249174896956522</v>
       </c>
       <c r="AK23">
-        <v>0.6665933240691972</v>
+        <v>0.666593324173913</v>
       </c>
       <c r="AL23">
-        <v>0.7082691585605476</v>
+        <v>0.7082691586521739</v>
       </c>
       <c r="AM23">
-        <v>0.7499449930518979</v>
+        <v>0.7499449931304347</v>
       </c>
       <c r="AN23">
-        <v>0.7916208275432484</v>
+        <v>0.7916208276086957</v>
       </c>
       <c r="AO23">
-        <v>0.8332966620345986</v>
+        <v>0.8332966620869565</v>
       </c>
       <c r="AP23">
-        <v>0.874972496525949</v>
+        <v>0.8749724965652174</v>
       </c>
       <c r="AQ23">
-        <v>0.9166483310172993</v>
+        <v>0.9166483310434782</v>
       </c>
       <c r="AR23">
-        <v>0.9583241655086497</v>
+        <v>0.9583241655217392</v>
       </c>
       <c r="AS23">
         <v>1</v>
@@ -35195,73 +35195,73 @@
         <v>0</v>
       </c>
       <c r="W24">
-        <v>0.0372169195679379</v>
+        <v>0.03721691956521739</v>
       </c>
       <c r="X24">
-        <v>0.0744338391358758</v>
+        <v>0.07443383913043478</v>
       </c>
       <c r="Y24">
-        <v>0.1116507587038137</v>
+        <v>0.1116507586956522</v>
       </c>
       <c r="Z24">
-        <v>0.1488676782717516</v>
+        <v>0.1488676782608696</v>
       </c>
       <c r="AA24">
-        <v>0.1860845978396895</v>
+        <v>0.1860845978260869</v>
       </c>
       <c r="AB24">
-        <v>0.2233015174076274</v>
+        <v>0.2233015173913043</v>
       </c>
       <c r="AC24">
-        <v>0.2605184369755653</v>
+        <v>0.2605184369565218</v>
       </c>
       <c r="AD24">
-        <v>0.2977353565435032</v>
+        <v>0.2977353565217391</v>
       </c>
       <c r="AE24">
-        <v>0.3349522761114411</v>
+        <v>0.3349522760869565</v>
       </c>
       <c r="AF24">
-        <v>0.372169195679379</v>
+        <v>0.3721691956521739</v>
       </c>
       <c r="AG24">
-        <v>0.4093861152473169</v>
+        <v>0.4093861152173913</v>
       </c>
       <c r="AH24">
-        <v>0.4466030348152548</v>
+        <v>0.4466030347826087</v>
       </c>
       <c r="AI24">
-        <v>0.4838199543831926</v>
+        <v>0.483819954347826</v>
       </c>
       <c r="AJ24">
-        <v>0.5210368739511306</v>
+        <v>0.5210368739130435</v>
       </c>
       <c r="AK24">
-        <v>0.5582537935190686</v>
+        <v>0.5582537934782609</v>
       </c>
       <c r="AL24">
-        <v>0.5954707130870064</v>
+        <v>0.5954707130434782</v>
       </c>
       <c r="AM24">
-        <v>0.6326876326549442</v>
+        <v>0.6326876326086955</v>
       </c>
       <c r="AN24">
-        <v>0.6699045522228823</v>
+        <v>0.6699045521739131</v>
       </c>
       <c r="AO24">
-        <v>0.7071214717908201</v>
+        <v>0.7071214717391304</v>
       </c>
       <c r="AP24">
-        <v>0.744338391358758</v>
+        <v>0.7443383913043478</v>
       </c>
       <c r="AQ24">
-        <v>0.7815553109266958</v>
+        <v>0.7815553108695652</v>
       </c>
       <c r="AR24">
-        <v>0.8187722304946339</v>
+        <v>0.8187722304347826</v>
       </c>
       <c r="AS24">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
     </row>
     <row r="25" spans="1:45">
@@ -35281,109 +35281,109 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="K25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="L25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="M25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="N25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="O25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="P25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="Q25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="R25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="S25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="T25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="U25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="V25">
-        <v>0.8559891500625717</v>
+        <v>0.85598915</v>
       </c>
       <c r="W25">
-        <v>0.8187722304946339</v>
+        <v>0.8187722304347826</v>
       </c>
       <c r="X25">
-        <v>0.7815553109266959</v>
+        <v>0.7815553108695652</v>
       </c>
       <c r="Y25">
-        <v>0.744338391358758</v>
+        <v>0.7443383913043478</v>
       </c>
       <c r="Z25">
-        <v>0.7071214717908201</v>
+        <v>0.7071214717391304</v>
       </c>
       <c r="AA25">
-        <v>0.6699045522228823</v>
+        <v>0.6699045521739131</v>
       </c>
       <c r="AB25">
-        <v>0.6326876326549442</v>
+        <v>0.6326876326086955</v>
       </c>
       <c r="AC25">
-        <v>0.5954707130870064</v>
+        <v>0.5954707130434782</v>
       </c>
       <c r="AD25">
-        <v>0.5582537935190686</v>
+        <v>0.5582537934782609</v>
       </c>
       <c r="AE25">
-        <v>0.5210368739511306</v>
+        <v>0.5210368739130435</v>
       </c>
       <c r="AF25">
-        <v>0.4838199543831928</v>
+        <v>0.4838199543478262</v>
       </c>
       <c r="AG25">
-        <v>0.4466030348152548</v>
+        <v>0.4466030347826087</v>
       </c>
       <c r="AH25">
-        <v>0.4093861152473169</v>
+        <v>0.4093861152173913</v>
       </c>
       <c r="AI25">
-        <v>0.3721691956793791</v>
+        <v>0.3721691956521739</v>
       </c>
       <c r="AJ25">
-        <v>0.3349522761114411</v>
+        <v>0.3349522760869565</v>
       </c>
       <c r="AK25">
-        <v>0.2977353565435032</v>
+        <v>0.2977353565217391</v>
       </c>
       <c r="AL25">
-        <v>0.2605184369755653</v>
+        <v>0.2605184369565218</v>
       </c>
       <c r="AM25">
-        <v>0.2233015174076274</v>
+        <v>0.2233015173913044</v>
       </c>
       <c r="AN25">
-        <v>0.1860845978396895</v>
+        <v>0.1860845978260869</v>
       </c>
       <c r="AO25">
-        <v>0.1488676782717516</v>
+        <v>0.1488676782608696</v>
       </c>
       <c r="AP25">
-        <v>0.1116507587038137</v>
+        <v>0.1116507586956522</v>
       </c>
       <c r="AQ25">
-        <v>0.07443383913587584</v>
+        <v>0.07443383913043483</v>
       </c>
       <c r="AR25">
-        <v>0.03721691956793788</v>
+        <v>0.03721691956521737</v>
       </c>
       <c r="AS25">
         <v>0</v>

</xml_diff>